<commit_message>
Wyniki eksperymentow dla sieci 50
</commit_message>
<xml_diff>
--- a/SenseSim-doc/projekt-raportu-komunikacji.xlsx
+++ b/SenseSim-doc/projekt-raportu-komunikacji.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michal/Documents/Workspace/SenseSim/SenseSim-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D64CA764-A8B2-7240-9A2D-33BC56310D58}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5666C98F-DE98-F842-B546-CE99A05BEF33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{0E08B154-22D1-BA4D-BE03-2247D360714B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" xr2:uid="{0E08B154-22D1-BA4D-BE03-2247D360714B}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>simTimeEnd</t>
   </si>
   <si>
-    <t>messageType</t>
-  </si>
-  <si>
     <t>messageContent</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>commStatus</t>
+  </si>
+  <si>
+    <t>commTime</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,25 +429,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
@@ -455,5 +455,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>